<commit_message>
Added to grading and readme
</commit_message>
<xml_diff>
--- a/SOEN287A3Grading.xlsx
+++ b/SOEN287A3Grading.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\Desktop\SOEN_287_A1\SOEN-287\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamo\Documents\GitHub\SOEN-287\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{995AA68F-4E9C-4135-A85A-B79D5BE429BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5D9BE7-0076-4ACC-A871-A2091283EAA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="17150" windowHeight="15950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>s</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>40153500,Kunal H. Shah</t>
+  </si>
+  <si>
+    <t>40174716, Adamo Orsini</t>
   </si>
 </sst>
 </file>
@@ -585,58 +588,58 @@
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -980,45 +983,45 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="20.100000000000001" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="20.149999999999999" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="56" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="41.7265625" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:8" ht="20.149999999999999" customHeight="1">
+      <c r="A1" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-    </row>
-    <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.149999999999999" customHeight="1">
+      <c r="A2" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-    </row>
-    <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A3" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="4" spans="1:8" ht="20.149999999999999" customHeight="1" thickBot="1">
       <c r="A4" s="3"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="5" spans="1:8" ht="20.149999999999999" customHeight="1" thickBot="1">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
@@ -1032,15 +1035,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:8" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A6" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="30"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="25"/>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="1:8" ht="81.95" customHeight="1" thickBot="1">
+    <row r="7" spans="1:8" ht="82" customHeight="1" thickBot="1">
       <c r="A7" s="11" t="s">
         <v>32</v>
       </c>
@@ -1050,15 +1053,15 @@
       <c r="C7" s="8"/>
       <c r="E7" s="17"/>
     </row>
-    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A8" s="29" t="s">
+    <row r="8" spans="1:8" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A8" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="30"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="25"/>
       <c r="E8" s="20"/>
     </row>
-    <row r="9" spans="1:8" ht="63.95" customHeight="1" thickBot="1">
+    <row r="9" spans="1:8" ht="64" customHeight="1" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>34</v>
       </c>
@@ -1068,18 +1071,18 @@
       <c r="C9" s="8"/>
       <c r="E9" s="17"/>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A10" s="29" t="s">
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A10" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="30"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="25"/>
       <c r="E10" s="20"/>
       <c r="H10" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="68.099999999999994" customHeight="1" thickBot="1">
+    <row r="11" spans="1:8" ht="68.150000000000006" customHeight="1" thickBot="1">
       <c r="A11" s="11" t="s">
         <v>35</v>
       </c>
@@ -1089,11 +1092,11 @@
       <c r="C11" s="8"/>
       <c r="E11" s="17"/>
     </row>
-    <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A12" s="29" t="s">
+    <row r="12" spans="1:8" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A12" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="30"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="25"/>
       <c r="E12" s="20"/>
     </row>
@@ -1107,15 +1110,17 @@
       <c r="C13" s="8"/>
       <c r="E13" s="17"/>
     </row>
-    <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A14" s="29" t="s">
+    <row r="14" spans="1:8" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A14" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="25"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="25" t="s">
+        <v>51</v>
+      </c>
       <c r="E14" s="20"/>
     </row>
-    <row r="15" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1">
+    <row r="15" spans="1:8" ht="40" customHeight="1" thickBot="1">
       <c r="A15" s="11" t="s">
         <v>37</v>
       </c>
@@ -1125,12 +1130,14 @@
       <c r="C15" s="8"/>
       <c r="E15" s="17"/>
     </row>
-    <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A16" s="29" t="s">
+    <row r="16" spans="1:8" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A16" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="25"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="25" t="s">
+        <v>51</v>
+      </c>
       <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:5" ht="39" customHeight="1" thickBot="1">
@@ -1143,17 +1150,17 @@
       <c r="C17" s="8"/>
       <c r="E17" s="17"/>
     </row>
-    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A18" s="29" t="s">
+    <row r="18" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A18" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="30"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="27" t="s">
         <v>50</v>
       </c>
       <c r="E18" s="20"/>
     </row>
-    <row r="19" spans="1:5" ht="48.95" customHeight="1" thickBot="1">
+    <row r="19" spans="1:5" ht="49" customHeight="1" thickBot="1">
       <c r="A19" s="12" t="s">
         <v>39</v>
       </c>
@@ -1163,17 +1170,17 @@
       <c r="C19" s="28"/>
       <c r="E19" s="17"/>
     </row>
-    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A20" s="29" t="s">
+    <row r="20" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A20" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="30"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="25" t="s">
         <v>50</v>
       </c>
       <c r="E20" s="20"/>
     </row>
-    <row r="21" spans="1:5" ht="35.1" customHeight="1" thickBot="1">
+    <row r="21" spans="1:5" ht="35.15" customHeight="1" thickBot="1">
       <c r="A21" s="11" t="s">
         <v>40</v>
       </c>
@@ -1183,15 +1190,15 @@
       <c r="C21" s="8"/>
       <c r="E21" s="17"/>
     </row>
-    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A22" s="29" t="s">
+    <row r="22" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A22" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="30"/>
+      <c r="B22" s="46"/>
       <c r="C22" s="25"/>
       <c r="E22" s="20"/>
     </row>
-    <row r="23" spans="1:5" ht="79.5" thickBot="1">
+    <row r="23" spans="1:5" ht="62.5" thickBot="1">
       <c r="A23" s="12" t="s">
         <v>41</v>
       </c>
@@ -1201,15 +1208,15 @@
       <c r="C23" s="8"/>
       <c r="E23" s="17"/>
     </row>
-    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A24" s="29" t="s">
+    <row r="24" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A24" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="30"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="25"/>
       <c r="E24" s="20"/>
     </row>
-    <row r="25" spans="1:5" ht="54.95" customHeight="1" thickBot="1">
+    <row r="25" spans="1:5" ht="55" customHeight="1" thickBot="1">
       <c r="A25" s="11" t="s">
         <v>42</v>
       </c>
@@ -1219,15 +1226,17 @@
       <c r="C25" s="8"/>
       <c r="E25" s="17"/>
     </row>
-    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A26" s="29" t="s">
+    <row r="26" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A26" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="25"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="25" t="s">
+        <v>51</v>
+      </c>
       <c r="E26" s="20"/>
     </row>
-    <row r="27" spans="1:5" ht="51.95" customHeight="1" thickBot="1">
+    <row r="27" spans="1:5" ht="52" customHeight="1" thickBot="1">
       <c r="A27" s="12" t="s">
         <v>43</v>
       </c>
@@ -1237,15 +1246,15 @@
       <c r="C27" s="8"/>
       <c r="E27" s="17"/>
     </row>
-    <row r="28" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A28" s="29" t="s">
+    <row r="28" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A28" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="30"/>
+      <c r="B28" s="46"/>
       <c r="C28" s="25"/>
       <c r="E28" s="20"/>
     </row>
-    <row r="29" spans="1:5" ht="59.1" customHeight="1" thickBot="1">
+    <row r="29" spans="1:5" ht="59.15" customHeight="1" thickBot="1">
       <c r="A29" s="11" t="s">
         <v>44</v>
       </c>
@@ -1255,11 +1264,11 @@
       <c r="C29" s="8"/>
       <c r="E29" s="17"/>
     </row>
-    <row r="30" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A30" s="29" t="s">
+    <row r="30" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A30" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="30"/>
+      <c r="B30" s="46"/>
       <c r="C30" s="25"/>
       <c r="E30" s="15"/>
     </row>
@@ -1273,13 +1282,13 @@
       <c r="C31" s="16"/>
     </row>
     <row r="32" spans="1:5" ht="21" customHeight="1" thickBot="1">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="35"/>
-    </row>
-    <row r="33" spans="1:5" ht="18.95" customHeight="1" thickBot="1">
+      <c r="B32" s="32"/>
+      <c r="C32" s="33"/>
+    </row>
+    <row r="33" spans="1:5" ht="19" customHeight="1" thickBot="1">
       <c r="A33" s="22" t="s">
         <v>21</v>
       </c>
@@ -1289,22 +1298,22 @@
       <c r="C33" s="14"/>
       <c r="E33" s="13"/>
     </row>
-    <row r="34" spans="1:5" ht="18.95" customHeight="1" thickBot="1">
-      <c r="A34" s="45" t="s">
+    <row r="34" spans="1:5" ht="19" customHeight="1" thickBot="1">
+      <c r="A34" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="46"/>
+      <c r="B34" s="44"/>
       <c r="C34" s="13"/>
       <c r="E34" s="15"/>
     </row>
-    <row r="35" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A35" s="39" t="s">
+    <row r="35" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A35" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="40"/>
+      <c r="B35" s="38"/>
       <c r="C35" s="18"/>
     </row>
-    <row r="36" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="36" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1">
       <c r="A36" s="21" t="s">
         <v>24</v>
       </c>
@@ -1313,21 +1322,21 @@
       </c>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A37" s="41" t="s">
+    <row r="37" spans="1:5" ht="20.149999999999999" customHeight="1">
+      <c r="A37" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="42"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="15"/>
     </row>
-    <row r="38" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A38" s="43" t="s">
+    <row r="38" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A38" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="44"/>
+      <c r="B38" s="42"/>
       <c r="C38" s="18"/>
     </row>
-    <row r="39" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="39" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1">
       <c r="A39" s="21" t="s">
         <v>26</v>
       </c>
@@ -1336,20 +1345,20 @@
       </c>
       <c r="C39" s="15"/>
     </row>
-    <row r="40" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A40" s="36" t="s">
+    <row r="40" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A40" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="37"/>
+      <c r="B40" s="35"/>
     </row>
     <row r="41" spans="1:5" ht="21" customHeight="1" thickBot="1">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="34"/>
-      <c r="C41" s="35"/>
-    </row>
-    <row r="42" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B41" s="32"/>
+      <c r="C41" s="33"/>
+    </row>
+    <row r="42" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1">
       <c r="A42" s="21" t="s">
         <v>46</v>
       </c>
@@ -1359,14 +1368,21 @@
       <c r="C42" s="25"/>
     </row>
     <row r="43" spans="1:5" ht="90" customHeight="1" thickBot="1">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="32"/>
+      <c r="B43" s="30"/>
     </row>
   </sheetData>
   <sheetProtection formatRows="0"/>
   <mergeCells count="23">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A40:B40"/>
@@ -1383,13 +1399,6 @@
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A41" r:id="rId1" display="file:///w/criteria" xr:uid="{0E378B40-F7DE-144E-90FF-1A1C56CABF87}"/>

</xml_diff>